<commit_message>
New changes to the FAIRe NOAA data model are now reflected in the code
</commit_message>
<xml_diff>
--- a/input/FAIRe_NOAA_checklist_v1.0.2.xlsx
+++ b/input/FAIRe_NOAA_checklist_v1.0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FA93413-2751-43B6-B381-2CD608EA4F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5D5462F-083D-4240-AA55-AD373EC89853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2373,7 +2373,7 @@
     <t>https://w3id.org/mixs/0001156</t>
   </si>
   <si>
-    <t>projectMetadata | experimentRunMetadata</t>
+    <t>projectMetadata | NOAAexperimentRunMetadata</t>
   </si>
   <si>
     <t>platform</t>
@@ -5310,8 +5310,8 @@
   <dimension ref="A1:P410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J303" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M312" sqref="M312"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A192" sqref="A192"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>